<commit_message>
att update status verification
</commit_message>
<xml_diff>
--- a/Planilhas/SALAS.xlsx
+++ b/Planilhas/SALAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\013190873\Downloads\Pessoal\VS\BB_Py_Automation\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29322843-B5D8-42D9-B362-596CFB29B056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C23A5804-135B-4133-8558-D4BA32BA22A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,57 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>STATUS</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_32</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_35</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_36</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_37</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_38</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_41</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_42</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_43</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_45</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_46</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_47</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_50</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_52</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_54</t>
-  </si>
-  <si>
-    <t>EAD_ENG_PROD_55</t>
   </si>
   <si>
     <t>ID_DESTINY</t>
@@ -687,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,81 +660,6 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -803,10 +683,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -833,634 +713,634 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B71" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B76" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B77" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B78" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B79" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update xlsx console utf-8
</commit_message>
<xml_diff>
--- a/Planilhas/SALAS.xlsx
+++ b/Planilhas/SALAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\013190873\Downloads\Pessoal\VS\BB_Py_Automation\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4EAEC0-A75F-48BC-8C65-B5845005972D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E22E71F-03F9-47B9-887D-173174D22D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,25 @@
     <sheet name="salaCopia" sheetId="2" r:id="rId2"/>
     <sheet name="atividades" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="126">
   <si>
     <t>ID</t>
   </si>
@@ -30,6 +43,93 @@
     <t>STATUS</t>
   </si>
   <si>
+    <t>LOG_RESULT</t>
+  </si>
+  <si>
+    <t>Fórum de Interação entre Professores e Tutores:</t>
+  </si>
+  <si>
+    <t>Meu Desempenho:</t>
+  </si>
+  <si>
+    <t>Organize seus estudos com a Sofia:</t>
+  </si>
+  <si>
+    <t>Fale com o Professor:</t>
+  </si>
+  <si>
+    <t>Desafio Colaborativo:</t>
+  </si>
+  <si>
+    <t>Unidade 1:</t>
+  </si>
+  <si>
+    <t>Unidade 2:</t>
+  </si>
+  <si>
+    <t>Unidade 3:</t>
+  </si>
+  <si>
+    <t>Unidade 4:</t>
+  </si>
+  <si>
+    <t>Material Didático Interativo from Unidade 1 :</t>
+  </si>
+  <si>
+    <t>Material Didático Interativo from Unidade 2 :</t>
+  </si>
+  <si>
+    <t>Material Didático Interativo from Unidade 3 :</t>
+  </si>
+  <si>
+    <t>Material Didático Interativo from Unidade 4 :</t>
+  </si>
+  <si>
+    <t>Videoteca: Videoaula from Unidade 1 :</t>
+  </si>
+  <si>
+    <t>Videoteca: Videoaula from Unidade 2 :</t>
+  </si>
+  <si>
+    <t>Videoteca: Videoaula from Unidade 3 :</t>
+  </si>
+  <si>
+    <t>Videoteca: Videoaula from Unidade 4 :</t>
+  </si>
+  <si>
+    <t>Biblioteca Virtual: e-Book from Unidade 1 :</t>
+  </si>
+  <si>
+    <t>Biblioteca Virtual: e-Book from Unidade 2 :</t>
+  </si>
+  <si>
+    <t>Biblioteca Virtual: e-Book from Unidade 3 :</t>
+  </si>
+  <si>
+    <t>Biblioteca Virtual: e-Book from Unidade 4 :</t>
+  </si>
+  <si>
+    <t>Atividade de Autoaprendizagem 1:</t>
+  </si>
+  <si>
+    <t>Atividade de Autoaprendizagem 2:</t>
+  </si>
+  <si>
+    <t>Atividade de Autoaprendizagem 3:</t>
+  </si>
+  <si>
+    <t>Atividade de Autoaprendizagem 4:</t>
+  </si>
+  <si>
+    <t>WebAula:</t>
+  </si>
+  <si>
+    <t>Solicite seu livro impresso:</t>
+  </si>
+  <si>
+    <t>SER Melhor (Clique Aqui para deixar seu elogio, crítica ou sugestão):</t>
+  </si>
+  <si>
     <t>ID_DESTINY</t>
   </si>
   <si>
@@ -313,9 +413,6 @@
   </si>
   <si>
     <t>Service Design</t>
-  </si>
-  <si>
-    <t>LOG_RESULT</t>
   </si>
 </sst>
 </file>
@@ -365,16 +462,129 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="32">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" wrapText="1"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -388,11 +598,107 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela1" displayName="Tabela1" ref="A1:B79" totalsRowShown="0">
-  <autoFilter ref="A1:B79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="A1:AE2" totalsRowShown="0" dataDxfId="31">
+  <autoFilter ref="A1:AE2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="STATUS" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="LOG_RESULT" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Fórum de Interação entre Professores e Tutores:" dataDxfId="27">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$D$1),$E$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Meu Desempenho:" dataDxfId="26">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$E$1),$F$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Organize seus estudos com a Sofia:" dataDxfId="25">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$F$1),$G$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Fale com o Professor:" dataDxfId="24">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$G$1),$H$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Desafio Colaborativo:" dataDxfId="23">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$H$1),$I$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Unidade 1:" dataDxfId="22">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$I$1),$J$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Unidade 2:" dataDxfId="21">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$J$1),$K$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Unidade 3:" dataDxfId="20">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$K$1),$L$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Unidade 4:" dataDxfId="19">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$L$1),$M$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Material Didático Interativo from Unidade 1 :" dataDxfId="18">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$M$1),$N$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Material Didático Interativo from Unidade 2 :" dataDxfId="17">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$N$1),$O$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Material Didático Interativo from Unidade 3 :" dataDxfId="16">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$O$1),$P$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Material Didático Interativo from Unidade 4 :" dataDxfId="15">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$P$1),$Q$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Videoteca: Videoaula from Unidade 1 :" dataDxfId="14">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$Q$1),$R$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Videoteca: Videoaula from Unidade 2 :" dataDxfId="13">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$R$1),$S$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Videoteca: Videoaula from Unidade 3 :" dataDxfId="12">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$S$1),$T$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Videoteca: Videoaula from Unidade 4 :" dataDxfId="11">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$T$1),$U$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Biblioteca Virtual: e-Book from Unidade 1 :" dataDxfId="10">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$U$1),$V$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Biblioteca Virtual: e-Book from Unidade 2 :" dataDxfId="9">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$V$1),$W$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Biblioteca Virtual: e-Book from Unidade 3 :" dataDxfId="8">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$W$1),$X$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Biblioteca Virtual: e-Book from Unidade 4 :" dataDxfId="7">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$X$1),$Y$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Atividade de Autoaprendizagem 1:" dataDxfId="6">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$Y$1),$Z$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Atividade de Autoaprendizagem 2:" dataDxfId="5">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$Z$1),$AA$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Atividade de Autoaprendizagem 3:" dataDxfId="4">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AA$1),$AB$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Atividade de Autoaprendizagem 4:" dataDxfId="3">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AB$1),$AC$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="WebAula:" dataDxfId="2">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AC$1),$AD$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Solicite seu livro impresso:" dataDxfId="1">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AD$1),$AE$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="SER Melhor (Clique Aqui para deixar seu elogio, crítica ou sugestão):" dataDxfId="0">
+      <calculatedColumnFormula>IFERROR(_xlfn.TEXTAFTER(TRIM(C2),$AE$1),"NOT FOUND")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabela1" displayName="Tabela1" ref="A1:B79" totalsRowShown="0">
+  <autoFilter ref="A1:B79" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="CURSO"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="GRANDE ÁREA"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CURSO"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="GRANDE ÁREA"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -661,20 +967,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="16" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="69.42578125" customWidth="1"/>
+    <col min="18" max="18" width="70" customWidth="1"/>
+    <col min="19" max="19" width="68.85546875" customWidth="1"/>
+    <col min="20" max="20" width="69.7109375" customWidth="1"/>
+    <col min="21" max="21" width="46" customWidth="1"/>
+    <col min="22" max="23" width="42.7109375" customWidth="1"/>
+    <col min="24" max="24" width="52.5703125" customWidth="1"/>
+    <col min="25" max="25" width="86.85546875" customWidth="1"/>
+    <col min="26" max="28" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.85546875" customWidth="1"/>
+    <col min="30" max="30" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,11 +1008,1074 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$D$1),$E$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$E$1),$F$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$F$1),$G$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$G$1),$H$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$H$1),$I$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$I$1),$J$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$J$1),$K$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$K$1),$L$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$L$1),$M$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$M$1),$N$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$N$1),$O$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$O$1),$P$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$P$1),$Q$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$Q$1),$R$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$R$1),$S$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$S$1),$T$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$T$1),$U$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$U$1),$V$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$V$1),$W$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$W$1),$X$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$X$1),$Y$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$Y$1),$Z$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$Z$1),$AA$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AA$1),$AB$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AB$1),$AC$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AC$1),$AD$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTBEFORE(_xlfn.TEXTAFTER(TRIM(C2),$AD$1),$AE$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="8">
+        <f ca="1">IFERROR(_xlfn.TEXTAFTER(TRIM(C2),$AE$1),"NOT FOUND")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+    </row>
+    <row r="4" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+    </row>
+    <row r="5" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+    </row>
+    <row r="6" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+    </row>
+    <row r="7" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+    </row>
+    <row r="8" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+    </row>
+    <row r="9" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+    </row>
+    <row r="10" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+    </row>
+    <row r="11" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+    </row>
+    <row r="12" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+    </row>
+    <row r="13" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="8"/>
+    </row>
+    <row r="14" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+    </row>
+    <row r="15" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="8"/>
+      <c r="AE15" s="8"/>
+    </row>
+    <row r="16" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
+    </row>
+    <row r="17" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="8"/>
+    </row>
+    <row r="18" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
+      <c r="AC18" s="8"/>
+      <c r="AD18" s="8"/>
+      <c r="AE18" s="8"/>
+    </row>
+    <row r="19" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AB19" s="8"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="8"/>
+    </row>
+    <row r="20" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+    </row>
+    <row r="21" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+    </row>
+    <row r="22" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="8"/>
+    </row>
+    <row r="23" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="8"/>
+    </row>
+    <row r="24" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+    </row>
+    <row r="25" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8"/>
+      <c r="AB25" s="8"/>
+      <c r="AC25" s="8"/>
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="8"/>
+    </row>
+    <row r="26" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8"/>
+      <c r="AE26" s="8"/>
+    </row>
+    <row r="27" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8"/>
+      <c r="Y27" s="8"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="8"/>
+      <c r="AB27" s="8"/>
+      <c r="AC27" s="8"/>
+      <c r="AD27" s="8"/>
+      <c r="AE27" s="8"/>
+    </row>
+    <row r="28" spans="1:31" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="8"/>
+      <c r="AB28" s="8"/>
+      <c r="AC28" s="8"/>
+      <c r="AD28" s="8"/>
+      <c r="AE28" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -706,10 +2095,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -717,8 +2106,6 @@
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9"/>
-      <c r="C9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -742,634 +2129,634 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="B53" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B55" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="B57" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="B58" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="B59" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>102</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>109</v>
       </c>
       <c r="B65" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="B66" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="B67" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>118</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
🐛 fix: Fixing a bug
</commit_message>
<xml_diff>
--- a/Planilhas/SALAS.xlsx
+++ b/Planilhas/SALAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\013190873\Downloads\Pessoal\VS\BB_Py_Automation\Planilhas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafad\Documents\vs\BB_Py_Automation\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CCEC727-0459-451E-BF33-C61633508AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{767DDDFA-E7AD-4C2B-8CA1-8717145F08C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="salas" sheetId="1" r:id="rId1"/>
@@ -375,7 +375,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -383,6 +383,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,42 +685,99 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="6"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+    </row>
+    <row r="4" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+    </row>
+    <row r="6" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+    </row>
+    <row r="7" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+    </row>
+    <row r="8" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+    </row>
+    <row r="9" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+    </row>
+    <row r="12" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+    </row>
+    <row r="16" spans="1:2" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+    </row>
+    <row r="18" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+    </row>
+    <row r="19" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+    </row>
+    <row r="21" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+    </row>
+    <row r="22" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+    </row>
+    <row r="24" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+    </row>
+    <row r="25" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+    </row>
+    <row r="26" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+    </row>
+    <row r="27" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+    </row>
+    <row r="28" spans="1:1" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="4294967294"/>

</xml_diff>